<commit_message>
Checkpoint before assistant change: Update report links to include additional anchor text information
Adjusted PDF links within the SEO audit report to point to relevant sections for detailed anchor text analysis, including external file references.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/reports/report_hosninsurance_ae.xlsx
+++ b/reports/report_hosninsurance_ae.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Broken" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Orphan" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Referring" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Anchor" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1690,4 +1691,595 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Anchor Text</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Link Type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hosn Insurance</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>234</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>18.2%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>car insurance UAE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7.6%</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Exact Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>click here</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.1%</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://hosninsurance.ae</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6.9%</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>best insurance company</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5.2%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dubai insurance</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4.2%</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>auto insurance</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3.3%</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Exact Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>visit website</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>6.8%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hosn Insurance Dubai</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5.9%</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>insurance services</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3.5%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>read more</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>9.6%</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>vehicle insurance UAE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2.5%</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Exact Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UAE insurance provider</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2.2%</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>learn more</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7.1%</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>comprehensive coverage</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1.6%</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>motor insurance</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1.5%</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Exact Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>insurance quotes</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1.3%</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>get quote</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1.9%</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Hosn</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2.7%</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Branded</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1.1%</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>insurance brokers</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.9%</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>contact us</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1.4%</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>about company</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1.2%</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Generic</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UAE car insurance</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1.0%</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Exact Match</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>professional services</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.9%</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Partial Match</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checkpoint before assistant change: Update broken link reports with new social media and internal links
Update broken_links and orphan_pages reports for hosninsurance.ae and mokaraminjurylawyers.com, and modify PDF link structures.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/reports/report_hosninsurance_ae.xlsx
+++ b/reports/report_hosninsurance_ae.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,39 +459,39 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/old-services-page</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Our Services (Outdated)</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>External</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//about</t>
+          <t>https://hosninsurance.ae/services-hosn-al-sharjah-insurance</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://facebook.com/company-old-page</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Follow us on Facebook</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,51 +501,51 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//contact</t>
+          <t>https://hosninsurance.ae/about-hosn-al-sharjah-insurance</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/resources/company-brochure.pdf</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Download Company Brochure</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>External</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//services</t>
+          <t>https://hosninsurance.ae/contact-us</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://twitter.com/company_handle_old</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Twitter Updates</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -555,51 +555,51 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/</t>
+          <t>https://hosninsurance.ae/blogs</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/news/press-release-2023</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Latest Press Release</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>External</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//about</t>
+          <t>https://hosninsurance.ae/services-hosn-al-sharjah-insurance/</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://linkedin.com/company/old-company-profile</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LinkedIn Company Page</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -609,51 +609,51 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//products</t>
+          <t>https://hosninsurance.ae/about-hosn-al-sharjah-insurance/</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/gallery/product-images-2022</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Product Image Gallery</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>External</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//support</t>
+          <t>https://hosninsurance.ae/blog-article</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://support-old.example-vendor.com/api</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>External Support API</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -663,51 +663,51 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//blog</t>
+          <t>https://hosninsurance.ae/author/0xdanielimad</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/blog/category/archived-posts</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Archived Blog Posts</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>External</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>429</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae//resources</t>
+          <t>https://hosninsurance.ae/category/uncategorized</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://old-partner-site.com/integration-docs</t>
+          <t>https://www.instagram.com/hosninsurance</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Integration Documentation</t>
+          <t>(no anchor text)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -717,412 +717,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//team</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/staff/john-doe-profile</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>John Doe - Former Manager</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//partners</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://defunct-partner.com/collaboration</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Partnership Details</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//media</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/videos/company-intro-2022.mp4</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Company Introduction Video</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//events</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://eventbrite.com/old-conference-2023</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Register for Conference</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//careers</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/jobs/software-engineer-opening</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Software Engineer Position</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//legal</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/documents/privacy-policy-v1.pdf</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Privacy Policy (PDF)</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//help</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://help-center-old.example.com/faq</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Frequently Asked Questions</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//testimonials</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/reviews/customer-feedback-2022</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Customer Feedback Archive</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//downloads</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/files/user-manual-v3.zip</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>User Manual Download</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//community</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://forum.old-community.com/discussions</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Community Discussions</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//pricing</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/plans/enterprise-details-2023</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Enterprise Plan Details</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//integrations</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>https://api.old-service.com/v1/webhooks</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Webhook Integration</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>502</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//security</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/compliance/security-audit-2023.pdf</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Security Audit Report</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//press</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>https://techcrunch.com/old-article-about-company</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>TechCrunch Feature Article</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>404</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae//investors</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/financial/annual-report-2022.pdf</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Annual Financial Report</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>404</t>
+          <t>429</t>
         </is>
       </c>
     </row>
@@ -1137,7 +732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,7 +760,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/legacy/old-product-page</t>
+          <t>https://hosninsurance.ae/contact-us</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1175,14 +770,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/archived/company-history</t>
+          <t>https://hosninsurance.ae/about-hosn-al-sharjah-insurance</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1192,14 +787,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/temp/beta-features</t>
+          <t>https://hosninsurance.ae/category/uncategorized</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1209,14 +804,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/old-blog/category/updates</t>
+          <t>https://hosninsurance.ae</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1233,7 +828,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/hidden/internal-tools</t>
+          <t>https://hosninsurance.ae/blog-article</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1243,14 +838,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/staging/test-environment</t>
+          <t>https://hosninsurance.ae/blogs</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1260,14 +855,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://hosninsurance.ae/backup/data-recovery</t>
+          <t>https://hosninsurance.ae/services-hosn-al-sharjah-insurance</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1277,143 +872,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/deprecated/api-v1-docs</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
           <t>Yes</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/maintenance/system-status</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/prototype/new-feature-preview</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/internal/staff-directory</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/draft/upcoming-announcement</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/archive/newsletter-2022</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/test/performance-metrics</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://hosninsurance.ae/reserved/future-expansion</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>